<commit_message>
updating for fingerprint demo
</commit_message>
<xml_diff>
--- a/test/testcases/testcase9_json_parquet_match.xlsx
+++ b/test/testcases/testcase9_json_parquet_match.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TigerAnalytics\accelerator\QE_Automated_Testing_Framework\test\testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D233E7D9-021B-4E37-9C73-199EE6EB4C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82564990-20A0-42CB-AC17-8E88C8A39052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>sourcequerymode</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>/app/test/s2t/source_json_target_parquet_s2t_9_match.xlsx</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -230,6 +233,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,14 +733,16 @@
       <c r="A32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="3">
-        <v>5</v>
+      <c r="B33" s="5">
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>